<commit_message>
Bill Of Materials (BOM) update
</commit_message>
<xml_diff>
--- a/Documentation/Materials.xlsx
+++ b/Documentation/Materials.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>ProtoScrewShield</t>
   </si>
@@ -208,13 +208,23 @@
   </si>
   <si>
     <t>AYZ0102AGRLC</t>
+  </si>
+  <si>
+    <t>Temperature sensor</t>
+  </si>
+  <si>
+    <t>TMP36</t>
+  </si>
+  <si>
+    <t>Adafruit/Sparkfun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -311,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -350,6 +360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -652,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +913,8 @@
         <v>5</v>
       </c>
       <c r="F12" s="13">
-        <v>3.75</v>
+        <f>1.44*E12</f>
+        <v>7.1999999999999993</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>36</v>
@@ -924,7 +936,8 @@
         <v>5</v>
       </c>
       <c r="F13" s="13">
-        <v>1.35</v>
+        <f>1.44*E13</f>
+        <v>7.1999999999999993</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>36</v>
@@ -1178,7 +1191,9 @@
       <c r="D26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="5">
+        <v>1</v>
+      </c>
       <c r="F26" s="13">
         <v>3</v>
       </c>
@@ -1187,22 +1202,44 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1</v>
+      </c>
+      <c r="F27" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="16">
-        <f>SUM(F3:F22)</f>
-        <v>221.78999999999996</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+      <c r="B29" s="16">
+        <f>SUM(F3:F22) + F27</f>
+        <v>232.58999999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="16">
-        <f>SUM(F3:F26)</f>
-        <v>245.07999999999996</v>
+      <c r="B30" s="16">
+        <f>SUM(F3:F27)</f>
+        <v>255.87999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>